<commit_message>
Created UML Use Case diagram of the different use cases so far, also added Exception use case for Creation of task, and added more alternate cases to the different use cases. Then added the GUI Sketches to RAD, adding more vocabulary and a bit more Non-functional requirements
</commit_message>
<xml_diff>
--- a/Documentation/Use Cases.xlsx
+++ b/Documentation/Use Cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\coffeebreak\coffeebreak\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\coffeebreak\coffeebreak\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Coffee Break</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Shows the Navigation Drawer with different categories</t>
   </si>
   <si>
-    <t>Picks a preferred category to filter out unwanted tasks</t>
-  </si>
-  <si>
     <t>Sets header to picked category's name, shows all tasks with picked filter</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>Takes user back to previous list of tasks, with the configured task updated in same place/order</t>
   </si>
   <si>
-    <t>Update/clean up list of done tasks</t>
-  </si>
-  <si>
     <t>Taps "More" button in top right corner</t>
   </si>
   <si>
@@ -150,6 +144,54 @@
   </si>
   <si>
     <t>Removes all checked off tasks withing the list</t>
+  </si>
+  <si>
+    <t>Picks a preferred time based category to show the tasks for that timespan</t>
+  </si>
+  <si>
+    <t>Picks a preferred  custom category to show the tasks with that label</t>
+  </si>
+  <si>
+    <t>Exception: Aborting creation of a Task</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.1.1</t>
+  </si>
+  <si>
+    <t>5.1.2</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>Begins to type in a name and then aborts by</t>
+  </si>
+  <si>
+    <t>Clicking the checkmark on the keyboard/outside the keyboard</t>
+  </si>
+  <si>
+    <t>Clicking the abort button</t>
+  </si>
+  <si>
+    <t>Aborts before clicking typing anything</t>
+  </si>
+  <si>
+    <t>6.1.1</t>
+  </si>
+  <si>
+    <t>6.1.2</t>
+  </si>
+  <si>
+    <t>Removes the task from the list</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Update/clean up list from completed tasks</t>
   </si>
 </sst>
 </file>
@@ -233,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -253,11 +295,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -274,11 +316,61 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -513,7 +605,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="D5:F13" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="D5:F13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <tableColumns count="3">
+    <tableColumn id="1" name="State" dataDxfId="27"/>
+    <tableColumn id="5" name="User" dataDxfId="26"/>
+    <tableColumn id="6" name="System" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell22" displayName="Tabell22" ref="H5:J7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="22"/>
     <tableColumn id="5" name="User" dataDxfId="21"/>
@@ -523,8 +626,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell22" displayName="Tabell22" ref="H5:J7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabell24" displayName="Tabell24" ref="D17:F24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="17"/>
     <tableColumn id="5" name="User" dataDxfId="16"/>
@@ -534,8 +637,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabell24" displayName="Tabell24" ref="D17:F23" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabell246" displayName="Tabell246" ref="D35:F40" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="12"/>
     <tableColumn id="5" name="User" dataDxfId="11"/>
@@ -545,8 +648,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabell246" displayName="Tabell246" ref="D28:F33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabell2467" displayName="Tabell2467" ref="H35:J39" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="7"/>
     <tableColumn id="5" name="User" dataDxfId="6"/>
@@ -556,8 +659,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabell2467" displayName="Tabell2467" ref="H28:J32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabell28" displayName="Tabell28" ref="H17:J30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="2"/>
     <tableColumn id="5" name="User" dataDxfId="1"/>
@@ -865,10 +968,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:X126"/>
+  <dimension ref="A1:X128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="H46:H47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +1044,7 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="3"/>
@@ -1096,6 +1199,10 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -1122,16 +1229,20 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="10" t="s">
-        <v>23</v>
+      <c r="D9" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8"/>
@@ -1148,16 +1259,20 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="10" t="s">
-        <v>24</v>
+      <c r="D10" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
@@ -1174,17 +1289,21 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>4</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="1"/>
@@ -1200,6 +1319,10 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1323,7 +1446,9 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="1"/>
@@ -1355,9 +1480,15 @@
         <v>4</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="H17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1377,7 +1508,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1385,9 +1516,13 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="7"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1407,7 +1542,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1415,9 +1550,13 @@
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="H19" s="7">
+        <v>2</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1445,9 +1584,13 @@
         <v>19</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="H20" s="7">
+        <v>3</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="7"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1467,17 +1610,21 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="7">
-        <v>3</v>
+      <c r="D21" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="H21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="7"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1493,21 +1640,25 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="7">
-        <v>4</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="H22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="7"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1523,21 +1674,25 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="H23" s="9">
+        <v>4</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1553,17 +1708,25 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="H24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="7"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1579,7 +1742,7 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1587,9 +1750,13 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="H25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="7"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1605,19 +1772,21 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="11"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="H26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="7"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1633,21 +1802,21 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="H27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="7"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1663,28 +1832,20 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>4</v>
+      <c r="H28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1704,22 +1865,18 @@
     <row r="29" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="7"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="10">
-        <v>1</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="7"/>
+      <c r="H29" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1735,24 +1892,20 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="10">
-        <v>2</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="10">
-        <v>2</v>
+      <c r="H30" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1769,25 +1922,17 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="7">
-        <v>3</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="7">
-        <v>3</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="7"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1803,25 +1948,19 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
     </row>
-    <row r="32" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="7">
-        <v>4</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="7"/>
+      <c r="C32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="7">
-        <v>4</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1837,21 +1976,17 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
     </row>
-    <row r="33" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="7">
-        <v>5</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1867,17 +2002,21 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="D34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="H34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -1897,13 +2036,25 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="D35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="H35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -1919,17 +2070,25 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="7"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="H36" s="9">
+        <v>1</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="7"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -1945,17 +2104,25 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="D37" s="9">
+        <v>2</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="H37" s="9">
+        <v>2</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -1971,17 +2138,25 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="D38" s="7">
+        <v>3</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="H38" s="7">
+        <v>3</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="7"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -1997,17 +2172,25 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="D39" s="7">
+        <v>4</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="7"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="H39" s="7">
+        <v>4</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2023,13 +2206,17 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="D40" s="7">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -4137,6 +4324,9 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
@@ -4160,6 +4350,9 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
@@ -4183,6 +4376,9 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
@@ -4206,6 +4402,9 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
@@ -4229,6 +4428,9 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
@@ -4245,16 +4447,46 @@
       <c r="X125" s="1"/>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+      <c r="T126" s="1"/>
+      <c r="U126" s="1"/>
+      <c r="V126" s="1"/>
+      <c r="W126" s="1"/>
+      <c r="X126" s="1"/>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C26:D26"/>
+  <mergeCells count="9">
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D4:F4"/>
@@ -4264,12 +4496,13 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalized UML Class Diagram and UML Use Cases
</commit_message>
<xml_diff>
--- a/Documentation/Use Cases.xlsx
+++ b/Documentation/Use Cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\coffeebreak\coffeebreak\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\coffeebreak\coffeebreak\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$D$5:$F$13</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Coffee Break</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Update/clean up list from completed tasks</t>
+  </si>
+  <si>
+    <t>5.1.3</t>
+  </si>
+  <si>
+    <t>Taping "Return"-button</t>
+  </si>
+  <si>
+    <t>6.1.3</t>
   </si>
 </sst>
 </file>
@@ -275,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -301,6 +310,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,12 +333,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,7 +650,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabell246" displayName="Tabell246" ref="D35:F40" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabell246" displayName="Tabell246" ref="D37:F42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="12"/>
     <tableColumn id="5" name="User" dataDxfId="11"/>
@@ -649,7 +661,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabell2467" displayName="Tabell2467" ref="H35:J39" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabell2467" displayName="Tabell2467" ref="H37:J41" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="7"/>
     <tableColumn id="5" name="User" dataDxfId="6"/>
@@ -660,7 +672,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabell28" displayName="Tabell28" ref="H17:J30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabell28" displayName="Tabell28" ref="H17:J32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" name="State" dataDxfId="2"/>
     <tableColumn id="5" name="User" dataDxfId="1"/>
@@ -970,8 +982,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:X128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,12 +997,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1014,10 +1026,10 @@
     </row>
     <row r="2" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1043,10 +1055,10 @@
     <row r="3" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="1"/>
@@ -1072,17 +1084,17 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1440,17 +1452,17 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1802,7 +1814,7 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
@@ -1811,10 +1823,10 @@
       <c r="F27" s="2"/>
       <c r="G27" s="1"/>
       <c r="H27" s="9" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="1"/>
@@ -1832,7 +1844,7 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
@@ -1841,12 +1853,12 @@
       <c r="F28" s="2"/>
       <c r="G28" s="1"/>
       <c r="H28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7" t="s">
-        <v>10</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="7"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1862,7 +1874,7 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
     </row>
-    <row r="29" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
@@ -1870,12 +1882,12 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16" t="s">
-        <v>52</v>
+      <c r="H29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1900,11 +1912,11 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7" t="s">
+      <c r="H30" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12" t="s">
         <v>52</v>
       </c>
       <c r="K30" s="1"/>
@@ -1922,7 +1934,7 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
@@ -1930,9 +1942,13 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="H31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1948,19 +1964,21 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
     </row>
-    <row r="32" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="H32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1976,17 +1994,17 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
     </row>
-    <row r="33" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2002,21 +2020,19 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2032,29 +2048,17 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2070,25 +2074,21 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" s="7"/>
+      <c r="D36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="9">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="7"/>
+      <c r="H36" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2104,24 +2104,28 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="9">
+      <c r="D37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7" t="s">
-        <v>31</v>
+      <c r="E37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="9">
+      <c r="H37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7" t="s">
-        <v>36</v>
+      <c r="I37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2138,23 +2142,23 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="7">
-        <v>3</v>
+      <c r="D38" s="9">
+        <v>1</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="7">
-        <v>3</v>
+      <c r="H38" s="9">
+        <v>1</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="1"/>
@@ -2172,24 +2176,24 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="7">
-        <v>4</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="7"/>
+      <c r="D39" s="9">
+        <v>2</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="7">
-        <v>4</v>
+      <c r="H39" s="9">
+        <v>2</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2206,21 +2210,25 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="7">
-        <v>5</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7" t="s">
-        <v>34</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="7"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="H40" s="7">
+        <v>3</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" s="7"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2236,17 +2244,25 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="D41" s="7">
+        <v>4</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="7"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="H41" s="7">
+        <v>4</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2262,13 +2278,17 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="D42" s="7">
+        <v>5</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -4476,17 +4496,22 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H36:J36"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D4:F4"/>

</xml_diff>

<commit_message>
Results from today's meeting
</commit_message>
<xml_diff>
--- a/Documentation/Use Cases.xlsx
+++ b/Documentation/Use Cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\coffeebreak\coffeebreak\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\coffeebreak\coffeebreak\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1222,8 +1222,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,7 +2492,7 @@
       <c r="W41" s="7"/>
       <c r="X41" s="7"/>
     </row>
-    <row r="42" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>

</xml_diff>